<commit_message>
Add planning excel file
</commit_message>
<xml_diff>
--- a/planning.xlsx
+++ b/planning.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marcelhacker/Documents/opensim-deadlift-techniques/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C192EBC-0601-A54C-B379-F019D323A704}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D81391C5-B218-FA40-971B-101BAF041458}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="680" yWindow="740" windowWidth="28040" windowHeight="16680" xr2:uid="{D596EE47-F267-354E-8852-8744F315EF1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="73">
-  <si>
-    <t>Test Athlete</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="75">
   <si>
     <t>Athlete 1</t>
   </si>
@@ -255,6 +252,15 @@
   </si>
   <si>
     <t>Email: marcel.hacker@univie.ac.at</t>
+  </si>
+  <si>
+    <t>Athlete 0</t>
+  </si>
+  <si>
+    <t>Inverse dynamics</t>
+  </si>
+  <si>
+    <t>Inverse kinematics</t>
   </si>
 </sst>
 </file>
@@ -335,23 +341,23 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -691,12 +697,12 @@
   <dimension ref="A1:M75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="22" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="19.1640625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="21.33203125" style="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="1" customWidth="1"/>
     <col min="3" max="3" width="17.1640625" style="1" customWidth="1"/>
     <col min="4" max="4" width="17" style="1" customWidth="1"/>
@@ -706,20 +712,20 @@
     <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="2"/>
       <c r="B1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>2</v>
       </c>
       <c r="E1" s="2"/>
       <c r="F1" s="2"/>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -729,7 +735,7 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -738,7 +744,9 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A4" s="2"/>
+      <c r="A4" s="2" t="s">
+        <v>74</v>
+      </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
@@ -746,7 +754,9 @@
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
+      <c r="A5" s="2" t="s">
+        <v>73</v>
+      </c>
       <c r="B5" s="2"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
@@ -754,28 +764,28 @@
       <c r="F5" s="2"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="I13" s="11" t="s">
-        <v>71</v>
-      </c>
-      <c r="J13" s="11"/>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11"/>
-      <c r="M13" s="11"/>
+      <c r="I13" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="J13" s="6"/>
+      <c r="K13" s="6"/>
+      <c r="L13" s="6"/>
+      <c r="M13" s="6"/>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="E14" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+        <v>68</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F14" s="7"/>
+      <c r="G14" s="7"/>
       <c r="I14" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="J14" s="10"/>
       <c r="K14" s="10"/>
@@ -783,332 +793,332 @@
       <c r="M14" s="10"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="6" t="s">
-        <v>6</v>
+      <c r="A15" s="4" t="s">
+        <v>5</v>
       </c>
       <c r="B15" s="1">
         <f>COUNTA(A15:A94)</f>
         <v>61</v>
       </c>
-      <c r="E15" s="7" t="s">
-        <v>68</v>
-      </c>
-      <c r="F15" s="7"/>
-      <c r="G15" s="7"/>
-      <c r="I15" s="3"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="3"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="E15" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="I15" s="11"/>
+      <c r="J15" s="11"/>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11"/>
+      <c r="M15" s="11"/>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E16" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
-      <c r="K16" s="3"/>
-      <c r="L16" s="3"/>
-      <c r="M16" s="3"/>
+      <c r="A16" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="E16" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="F16" s="9"/>
+      <c r="G16" s="9"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="11"/>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11"/>
+      <c r="M16" s="11"/>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="3" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A18" s="3" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A18" s="5" t="s">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A19" s="5" t="s">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A20" s="5" t="s">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A21" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A21" s="5" t="s">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A22" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A22" s="5" t="s">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A23" s="3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A23" s="5" t="s">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A24" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A24" s="5" t="s">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A25" s="5" t="s">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A26" s="5" t="s">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A27" s="3" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A27" s="5" t="s">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A28" s="4" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A28" s="6" t="s">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A29" s="4" t="s">
         <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A29" s="6" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A32" s="5" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A33" s="3" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A33" s="5" t="s">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A34" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A34" s="5" t="s">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A35" s="3" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A35" s="5" t="s">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A36" s="4" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A36" s="6" t="s">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A37" s="4" t="s">
         <v>28</v>
-      </c>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A37" s="6" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A38" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A39" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A40" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A40" s="9" t="s">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A41" s="3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A41" s="5" t="s">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A42" s="3" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A42" s="5" t="s">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A43" s="3" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A43" s="5" t="s">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A44" s="3" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A44" s="5" t="s">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A45" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A45" s="5" t="s">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A46" s="3" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A46" s="5" t="s">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A47" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A48" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A48" s="6" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A49" s="6" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A50" s="5" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" s="3" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A51" s="5" t="s">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A52" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A52" s="5" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A53" s="5" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A54" s="3" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A54" s="5" t="s">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A55" s="3" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A55" s="5" t="s">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A56" s="3" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A56" s="5" t="s">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A57" s="3" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A57" s="5" t="s">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A58" s="3" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A58" s="5" t="s">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" s="3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A59" s="5" t="s">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A60" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A60" s="5" t="s">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A61" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A61" s="5" t="s">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A62" s="3" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A62" s="5" t="s">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A63" s="3" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A63" s="5" t="s">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A64" s="4" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A64" s="6" t="s">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A65" s="4" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A65" s="6" t="s">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A66" s="3" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A66" s="5" t="s">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A67" s="3" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A67" s="5" t="s">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A68" s="3" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A68" s="5" t="s">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A69" s="3" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A69" s="5" t="s">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A70" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A70" s="5" t="s">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A71" s="3" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A71" s="5" t="s">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A72" s="3" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A72" s="5" t="s">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A73" s="3" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A73" s="5" t="s">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A74" s="3" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A74" s="5" t="s">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A75" s="3" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A75" s="5" t="s">
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>